<commit_message>
fix graduate confirmation, fix send mail graduate student
</commit_message>
<xml_diff>
--- a/04.Source/CapstoneMVC/src/main/resources/template/Xacnhan_TotNghiep.xlsx
+++ b/04.Source/CapstoneMVC/src/main/resources/template/Xacnhan_TotNghiep.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\StormNs\Desktop\my-excel\my-template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\IntelliJsWorkShop\Capstone\04.Source\CapstoneMVC\src\main\resources\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FA579DD2-0EE5-4B64-948D-F98EB7075027}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{71522711-3507-456E-90F7-25363DBBBD2D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{38290F07-C846-452E-B35D-87CBE8725003}"/>
   </bookViews>
@@ -468,7 +468,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14FD6F56-C898-420A-9BAE-BD0B909310D3}">
   <dimension ref="A3:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B3" sqref="B3:G3"/>
     </sheetView>
   </sheetViews>
@@ -477,7 +477,7 @@
     <col min="1" max="1" width="6.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="15.42578125" style="1" customWidth="1"/>
     <col min="3" max="3" width="9.140625" style="1"/>
-    <col min="4" max="4" width="19.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" style="1" customWidth="1"/>
     <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
add academic transcript print, fix template
</commit_message>
<xml_diff>
--- a/04.Source/CapstoneMVC/src/main/resources/template/Xacnhan_TotNghiep.xlsx
+++ b/04.Source/CapstoneMVC/src/main/resources/template/Xacnhan_TotNghiep.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\IntelliJsWorkShop\Capstone\04.Source\CapstoneMVC\src\main\resources\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{71522711-3507-456E-90F7-25363DBBBD2D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{B2DDFA40-C20B-4764-BB4E-F473C1B39E8E}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{38290F07-C846-452E-B35D-87CBE8725003}"/>
   </bookViews>
@@ -30,9 +30,6 @@
     <t>GIẤY XÁC NHẬN</t>
   </si>
   <si>
-    <t>Trường đại học FPT xác nhận</t>
-  </si>
-  <si>
     <t xml:space="preserve">Sinh viên: </t>
   </si>
   <si>
@@ -63,13 +60,16 @@
     <t>Quyết định</t>
   </si>
   <si>
-    <t>Tại trường đại học FPT.</t>
-  </si>
-  <si>
     <t>TP.HCM,</t>
   </si>
   <si>
-    <t xml:space="preserve">     TUQ. VIỆN TRƯỞNG</t>
+    <t>Trường Đại học FPT xác nhận</t>
+  </si>
+  <si>
+    <t>Tại trường Đại học FPT.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     T. VIỆN TRƯỞNG</t>
   </si>
 </sst>
 </file>
@@ -468,8 +468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14FD6F56-C898-420A-9BAE-BD0B909310D3}">
   <dimension ref="A3:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:G3"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -493,67 +493,67 @@
     </row>
     <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D21" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D23" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D25" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="30" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="F30" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="31" spans="2:6" ht="17.25" x14ac:dyDescent="0.3">

</xml_diff>